<commit_message>
Fix typos in instructions
</commit_message>
<xml_diff>
--- a/Aus/BOM Locations and Districts.xlsx
+++ b/Aus/BOM Locations and Districts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AmandaandDarryn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\weather-projects\weewx-responsive-skin\Aus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4555,12 +4555,6 @@
     <t>Once you select your locality you can then find out which District Forecast file to use</t>
   </si>
   <si>
-    <t xml:space="preserve">If there is one ID, then this is the ID for the Forecast product ID. If there is two IDs, one will be the Locaility ID, matching that shown above, </t>
-  </si>
-  <si>
-    <t>the other being the district Forceast product ID.</t>
-  </si>
-  <si>
     <t>Although it is not important what you call your District Forecast File in skin.conf, looking at the Detailed forecast page,</t>
   </si>
   <si>
@@ -4576,9 +4570,6 @@
     <t>…</t>
   </si>
   <si>
-    <t>For Buladehlah this is Min North Coast area, so you may name your District Forecast File MID_NORTH_COAST</t>
-  </si>
-  <si>
     <t>IDN11025</t>
   </si>
   <si>
@@ -4586,9 +4577,6 @@
   </si>
   <si>
     <t>MID_NORTH_COAST=ftp://ftp.bom.gov.au/anon/gen/fwo/IDN11025.xml</t>
-  </si>
-  <si>
-    <t>[[[fc_local]]</t>
   </si>
   <si>
     <t>[[xml_files]]</t>
@@ -4652,32 +4640,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Select your </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Localitiy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. This is the locaility name you need to use in Responsive skin.conf</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Click the </t>
     </r>
     <r>
@@ -4808,6 +4770,44 @@
   </si>
   <si>
     <t>NOTE: If you have a late version of Excel with Power Query, you can update the quries which drive all the State locality data which drive the spreadsheet</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select your </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Locality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. This is the locality name you need to use in Responsive skin.conf</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">If there is one ID, then this is the ID for the Forecast product ID. If there is two IDs, one will be the Locality ID, matching that shown above, </t>
+  </si>
+  <si>
+    <t>the other being the district Forecast product ID.</t>
+  </si>
+  <si>
+    <t>For Buladelah this is Min North Coast area, so you may name your District Forecast File MID_NORTH_COAST</t>
+  </si>
+  <si>
+    <t>[[fc_local]]</t>
   </si>
 </sst>
 </file>
@@ -5205,7 +5205,7 @@
     <tableColumn id="2" name="Table"/>
     <tableColumn id="5" name="Loclity_Product"/>
     <tableColumn id="4" name="Locality_File"/>
-    <tableColumn id="3" name="Locaility_Lookup" dataDxfId="29">
+    <tableColumn id="3" name="Locaility_Lookup" dataDxfId="1">
       <calculatedColumnFormula>CONCATENATE(STATE_LOOKUP[[#This Row],[Table]],"[Attribute:description]")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" name="Full_Table" dataDxfId="0">
@@ -5233,10 +5233,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="NSW" displayName="NSW" ref="A1:D143" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D143"/>
   <tableColumns count="4">
-    <tableColumn id="4" uniqueName="4" name="Attribute:description" queryTableFieldId="3" dataDxfId="28"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:aac" queryTableFieldId="2" dataDxfId="27"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:type" queryTableFieldId="4" dataDxfId="26"/>
-    <tableColumn id="6" uniqueName="6" name="Attribute:parent-aac" queryTableFieldId="5" dataDxfId="25"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:description" queryTableFieldId="3" dataDxfId="29"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:aac" queryTableFieldId="2" dataDxfId="28"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:type" queryTableFieldId="4" dataDxfId="27"/>
+    <tableColumn id="6" uniqueName="6" name="Attribute:parent-aac" queryTableFieldId="5" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5246,10 +5246,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="VIC" displayName="VIC" ref="A1:D85" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D85"/>
   <tableColumns count="4">
-    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="24"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="23"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="22"/>
-    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="25"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="24"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="23"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5259,10 +5259,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="QLD" displayName="QLD" ref="A1:D113" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D113"/>
   <tableColumns count="4">
-    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="12"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="11"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="21"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="20"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="19"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5272,10 +5272,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="SA" displayName="SA" ref="A1:D60" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D60"/>
   <tableColumns count="4">
-    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="15"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="14"/>
-    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="13"/>
+    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="16"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5285,10 +5285,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="WA" displayName="WA" ref="A1:D115" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D115"/>
   <tableColumns count="4">
-    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="7"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="6"/>
-    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="5"/>
+    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="13"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5298,10 +5298,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TAS" displayName="TAS" ref="A1:D71" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D71"/>
   <tableColumns count="4">
-    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="3"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="8"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="7"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5311,10 +5311,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="NT" displayName="NT" ref="A1:D97" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:D97"/>
   <tableColumns count="4">
-    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="20"/>
-    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="19"/>
-    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="18"/>
-    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="17"/>
+    <tableColumn id="2" uniqueName="2" name="Attribute:description" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="5" uniqueName="5" name="Attribute:aac" queryTableFieldId="1" dataDxfId="4"/>
+    <tableColumn id="3" uniqueName="3" name="Attribute:type" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" uniqueName="4" name="Attribute:parent-aac" queryTableFieldId="4" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5619,8 +5619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5688,7 +5688,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>1494</v>
+        <v>1491</v>
       </c>
       <c r="C6" s="2" t="str">
         <f>IF(ISTEXT(DistrcitTable[District Product]),HYPERLINK(CONCATENATE("ftp://ftp.bom.gov.au/anon/gen/fwo/",DistrcitTable[District Product],".xml")),"")</f>
@@ -5712,7 +5712,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>1504</v>
+        <v>1500</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -5730,7 +5730,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>1505</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -5738,7 +5738,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>1506</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -5754,7 +5754,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>1507</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -5762,7 +5762,7 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>1508</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -5770,7 +5770,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>1509</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -5778,12 +5778,12 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>1486</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>1487</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -5791,7 +5791,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>1510</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -5799,7 +5799,7 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>1511</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -5807,22 +5807,22 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
-        <v>1493</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>1495</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -5830,75 +5830,75 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>1498</v>
-      </c>
-      <c r="E50" t="s">
-        <v>1499</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C51" t="s">
-        <v>1491</v>
+        <v>1489</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1495</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C53" t="s">
-        <v>1496</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>1497</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C57" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C59" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
-        <v>1503</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -5906,7 +5906,7 @@
         <v>14</v>
       </c>
       <c r="B64" t="s">
-        <v>1512</v>
+        <v>1507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>